<commit_message>
Start of Rev 2 (using TIM2 for red) before chnging the TIM1 config
</commit_message>
<xml_diff>
--- a/Nucleo-G0B1RE_Header_Pinout_PDM_Driver4_Rev_2.xlsx
+++ b/Nucleo-G0B1RE_Header_Pinout_PDM_Driver4_Rev_2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\John\code\STM32CubeIDE\PBM_Device_Code\nucleo_G0B1RE_driver4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8289E9AA-6B76-438A-ACA0-DFAB9D3E3B97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F3266E8-1106-4652-9361-7305748876B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="169">
   <si>
     <t>MIT License</t>
   </si>
@@ -522,6 +522,12 @@
   </si>
   <si>
     <t>(UART2_TX)</t>
+  </si>
+  <si>
+    <t>LED1</t>
+  </si>
+  <si>
+    <t>LED2</t>
   </si>
 </sst>
 </file>
@@ -693,7 +699,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="22">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -817,6 +823,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1074,7 +1086,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1205,22 +1217,25 @@
     <xf numFmtId="0" fontId="21" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="20" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="13" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="21" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1251,6 +1266,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFCC99"/>
       <color rgb="FFC198E0"/>
       <color rgb="FF8A3CC4"/>
     </mruColors>
@@ -1861,7 +1877,7 @@
   <dimension ref="A1:W45"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W18" sqref="W18"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1960,7 +1976,7 @@
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="56" t="s">
         <v>157</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1976,10 +1992,10 @@
       <c r="H7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="56" t="s">
+      <c r="I7" s="55" t="s">
         <v>158</v>
       </c>
-      <c r="O7" s="56" t="s">
+      <c r="O7" s="55" t="s">
         <v>159</v>
       </c>
       <c r="P7" s="31"/>
@@ -1998,7 +2014,7 @@
       <c r="U7" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="V7" s="56" t="s">
+      <c r="V7" s="55" t="s">
         <v>160</v>
       </c>
     </row>
@@ -2221,7 +2237,7 @@
       <c r="H12" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="I12" s="58" t="s">
+      <c r="I12" s="57" t="s">
         <v>116</v>
       </c>
       <c r="M12" s="52"/>
@@ -2332,7 +2348,7 @@
       <c r="H14" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="I14" s="58" t="s">
+      <c r="I14" s="57" t="s">
         <v>116</v>
       </c>
       <c r="M14" s="4"/>
@@ -2437,7 +2453,7 @@
       <c r="H16" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I16" s="59" t="s">
+      <c r="I16" s="58" t="s">
         <v>33</v>
       </c>
       <c r="O16" s="14" t="s">
@@ -2461,7 +2477,7 @@
       <c r="U16" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="V16" s="59" t="s">
+      <c r="V16" s="58" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2487,7 +2503,7 @@
       <c r="H17" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="I17" s="58" t="s">
         <v>33</v>
       </c>
       <c r="O17" s="53" t="s">
@@ -2511,7 +2527,7 @@
       <c r="U17" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="V17" s="55" t="s">
+      <c r="V17" s="54" t="s">
         <v>164</v>
       </c>
     </row>
@@ -2644,8 +2660,8 @@
       <c r="H20" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="I20" s="54"/>
-      <c r="O20" s="55" t="s">
+      <c r="I20" s="14"/>
+      <c r="O20" s="54" t="s">
         <v>162</v>
       </c>
       <c r="P20" s="31" t="s">
@@ -2666,7 +2682,7 @@
       <c r="U20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="V20" s="54"/>
+      <c r="V20" s="14"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
@@ -2693,8 +2709,8 @@
       <c r="H21" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="I21" s="54"/>
-      <c r="O21" s="55" t="s">
+      <c r="I21" s="14"/>
+      <c r="O21" s="54" t="s">
         <v>161</v>
       </c>
       <c r="P21" s="31" t="s">
@@ -2747,7 +2763,7 @@
       <c r="I22" s="48" t="s">
         <v>138</v>
       </c>
-      <c r="O22" s="55" t="s">
+      <c r="O22" s="54" t="s">
         <v>163</v>
       </c>
       <c r="P22" s="31" t="s">
@@ -2768,7 +2784,7 @@
       <c r="U22" s="46" t="s">
         <v>104</v>
       </c>
-      <c r="V22" s="59" t="s">
+      <c r="V22" s="58" t="s">
         <v>33</v>
       </c>
     </row>
@@ -2795,7 +2811,7 @@
         <v>54</v>
       </c>
       <c r="I23" s="14"/>
-      <c r="O23" s="54"/>
+      <c r="O23" s="14"/>
       <c r="P23" s="31" t="s">
         <v>100</v>
       </c>
@@ -2843,7 +2859,9 @@
       <c r="H24" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="54"/>
+      <c r="I24" s="59" t="s">
+        <v>167</v>
+      </c>
       <c r="M24" s="3"/>
       <c r="O24" s="14" t="s">
         <v>48</v>
@@ -2892,8 +2910,8 @@
       <c r="H25" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="I25" s="20" t="s">
-        <v>156</v>
+      <c r="I25" s="60" t="s">
+        <v>168</v>
       </c>
       <c r="M25" s="3"/>
       <c r="O25" s="20" t="s">

</xml_diff>